<commit_message>
Ajout version révisée du registre de risque
</commit_message>
<xml_diff>
--- a/Remise/Remise 1/registre_risque.xlsx
+++ b/Remise/Remise 1/registre_risque.xlsx
@@ -1,30 +1,32 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="60" windowWidth="12915" windowHeight="9780"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
     <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
   <si>
     <t>Type de risque</t>
   </si>
   <si>
     <t>Probabilité d'occurrence</t>
-  </si>
-  <si>
-    <t>Responsible du risque</t>
   </si>
   <si>
     <t>Retard sur le projet</t>
@@ -52,10 +54,6 @@
  associé au risque</t>
   </si>
   <si>
-    <t>Délai de livraison
- du simulateur à temps réel non respecté</t>
-  </si>
-  <si>
     <t>Impossibilité de
  faire la simulation en temps réel</t>
   </si>
@@ -72,97 +70,11 @@
  dans l'équipe</t>
   </si>
   <si>
-    <t>Parler aux clients sur la suite des objectifs</t>
-  </si>
-  <si>
     <t>Niveau de priorité
 (1 faible, 5 élevé)</t>
   </si>
   <si>
-    <t xml:space="preserve">Tous les objectifs ne seront pas atteints
-</t>
-  </si>
-  <si>
     <t>Francis Valois</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bris de l'ordinateur
- utilisé pour les simulations </t>
-  </si>
-  <si>
-    <t xml:space="preserve">La simulation n'accepte pas certaines entrées </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pas de résultats pour la simulation 
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Incapacité de fournir un simulateur fonctionnel
-</t>
-  </si>
-  <si>
-    <t>Pas de licence de disponible pour MATLAB</t>
-  </si>
-  <si>
-    <t>Le simulateur avec simpowersystem ne peut pas ouvrir</t>
-  </si>
-  <si>
-    <t>Problème de communication entre les différentes sections de la simulation</t>
-  </si>
-  <si>
-    <t>Plusieurs heures avant une démonstration, ouvrir MATLAB</t>
-  </si>
-  <si>
-    <t>Faire des tests qui prend en compte tous les paramètres possibles et indiquer dans le support accompagnant le simulateur les entrées attendus</t>
-  </si>
-  <si>
-    <t>Prévoir un ordinateur de secours</t>
-  </si>
-  <si>
-    <t>La simulation n'émet pas de résultats</t>
-  </si>
-  <si>
-    <t>Tests rigureux sur les simulations des
- différentes plateformes</t>
-  </si>
-  <si>
-    <t>Incapacité de lancer les simulations</t>
-  </si>
-  <si>
-    <t>Les simulations
-ne fonctionnent pas</t>
-  </si>
-  <si>
-    <t>Tests rigureux des
-des simulations</t>
-  </si>
-  <si>
-    <t>Impossibilité d'obtenir
- des résultats des simulations</t>
-  </si>
-  <si>
-    <t>Incapacité de faire la validation croisée
- des simulateurs</t>
-  </si>
-  <si>
-    <t>Impossibilité de démontrer le fonctionnement du simulateur</t>
-  </si>
-  <si>
-    <t>Effaçage des 
-simulations</t>
-  </si>
-  <si>
-    <t>Incapacité de démontrer
-le fonctionnement 
-des simulations</t>
-  </si>
-  <si>
-    <t>Toujours garder plusieurs
-capies à jour des simulations</t>
-  </si>
-  <si>
-    <t>Les simulations ne
- sont plus disponible</t>
   </si>
   <si>
     <t>Utilisation 
@@ -173,36 +85,66 @@
 ne fonctionnent plus correctement </t>
   </si>
   <si>
-    <t>Les résultats des simulations sont incorrectes</t>
-  </si>
-  <si>
-    <t>Toujours garder plusieurs
-copies de la simulation de différentes étapes d'avancement</t>
-  </si>
-  <si>
-    <t>L'ordinateur ne veut plus démarrer</t>
-  </si>
-  <si>
-    <t>Cyberattaque aux ordinateurs du
- réseau de l'université laval</t>
-  </si>
-  <si>
-    <t xml:space="preserve">L'ordinateur ne répond plus </t>
-  </si>
-  <si>
-    <t>La simulation à
-temps réel est inopérable</t>
-  </si>
-  <si>
-    <t>S'assurer que les ordinateurs
-utilisé soit équipé d'une bonne protection par-feu</t>
+    <t>Délai de livraison
+ du simulateur en temps réel non respecté</t>
+  </si>
+  <si>
+    <t>Maintenir une communication efficace avec le LEEPCI dans l'optique de se servir du simulateur dès son arrivée</t>
+  </si>
+  <si>
+    <t>Pertes des données liées aux simulateurs</t>
+  </si>
+  <si>
+    <t>Retard sur le projet mineur s'il existe une révision récente et retards majeurs dans le cas échéant</t>
+  </si>
+  <si>
+    <t>Certains objectifs ne seront pas atteints dans les temps initiaux prescrits</t>
+  </si>
+  <si>
+    <t>S'assurer de bien maintenir les révisions à jour, travaille collaboratif mis fréquemment à jour et dont les changements sont réversibles au moyen d'une synchronisation sur un serveur web protégé (github)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Versions  de développement et d'utilisation différentes de Matlab </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Certaines fonctionnalités du simulateur en temps réel ne pourraient pas concorder, certains modules de simulink ou certaines fonctionnalités de Matlab pourraient ne pas être compatibles
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Incapacité de fournir un simulateur fonctionnant explicitement comme décrit dans la documentation, besoin d'effectuer des modifications internes importantes, du côté du client, pour maintenir le fonctionnement désiré du simulateur
+</t>
+  </si>
+  <si>
+    <t>Faire des tests à partir de différentes plateformes et à partir de différents systèmes d'exploitations de manière à s'assurer l'homogénité dans le fonctionnement de Matlab</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Disconcordance dans les versions de PSIM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Certaines fonctionnalités du simulateur implanté sur PSIM pourraient être différentes selon la version employée.
+</t>
+  </si>
+  <si>
+    <t>Différence dans les résultats produits à partir du simulateur implanté sur PSIM, il se peut que les résultats ne concordent plus avec les autres simulateurs</t>
+  </si>
+  <si>
+    <t>Tester le simulateur sur le plus différentes versions de PSIM</t>
+  </si>
+  <si>
+    <t>Responsable du risque</t>
+  </si>
+  <si>
+    <t>Toujours garder plusieurs copies de la simulation à différentes étapes du projet et limiter l'utilisateur dans les manipulations potentiellement néfastes pour le fonctionnement du simulateur (avertissements dans la documentation)</t>
+  </si>
+  <si>
+    <t>Le simulateur ne s'amorçe plus correctement, les affichages ne sont plus fonctionnels, les données ne concordent plus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -214,6 +156,22 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -237,50 +195,52 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="double">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -309,7 +269,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -609,93 +571,93 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
-    <col min="4" max="4" width="24.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" customWidth="1"/>
-    <col min="6" max="6" width="19.5703125" customWidth="1"/>
-    <col min="7" max="7" width="20.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.1640625" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.83203125" customWidth="1"/>
+    <col min="6" max="6" width="19.5" customWidth="1"/>
+    <col min="7" max="7" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="67.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="67.5" customHeight="1" thickBot="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C1" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="8" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>9</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>2</v>
+        <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="66" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="66" customHeight="1" thickTop="1">
       <c r="A2" s="4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="5">
         <v>1</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E2" s="6">
         <v>0.1</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G2" s="5" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="84">
+      <c r="A3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1">
+        <v>5</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1">
-        <v>3</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="3">
-        <v>0.7</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="66" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="154">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
@@ -703,185 +665,98 @@
         <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>45</v>
+        <v>20</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="E4" s="3">
         <v>0.2</v>
       </c>
       <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="154">
+      <c r="A5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="1">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.15</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="98">
+      <c r="A6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B6" s="1">
+        <v>3</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="137.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B5" s="1">
-        <v>5</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" s="3">
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="3">
         <v>0.1</v>
       </c>
-      <c r="F5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="71.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="1">
-        <v>5</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.05</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="94.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="168">
       <c r="A7" s="2" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="B7" s="1">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E7" s="3">
-        <v>0.05</v>
+        <v>0.2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B8" s="1">
-        <v>4</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="E8" s="3">
-        <v>0.2</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" s="1">
-        <v>5</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="E9" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="98.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="B10" s="1">
-        <v>5</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="3">
-        <v>0.15</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="81" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="B11" s="1">
-        <v>2</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="3">
-        <v>0.05</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -891,9 +766,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -903,8 +783,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correction du registre de risque
</commit_message>
<xml_diff>
--- a/Remise/Remise 1/registre_risque.xlsx
+++ b/Remise/Remise 1/registre_risque.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14160"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20440" windowHeight="14000"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="34">
   <si>
     <t>Type de risque</t>
   </si>
@@ -101,9 +101,6 @@
     <t>Certains objectifs ne seront pas atteints dans les temps initiaux prescrits</t>
   </si>
   <si>
-    <t>S'assurer de bien maintenir les révisions à jour, travaille collaboratif mis fréquemment à jour et dont les changements sont réversibles au moyen d'une synchronisation sur un serveur web protégé (github)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Versions  de développement et d'utilisation différentes de Matlab </t>
   </si>
   <si>
@@ -115,9 +112,6 @@
 </t>
   </si>
   <si>
-    <t>Faire des tests à partir de différentes plateformes et à partir de différents systèmes d'exploitations de manière à s'assurer l'homogénité dans le fonctionnement de Matlab</t>
-  </si>
-  <si>
     <t xml:space="preserve">Disconcordance dans les versions de PSIM </t>
   </si>
   <si>
@@ -128,9 +122,6 @@
     <t>Différence dans les résultats produits à partir du simulateur implanté sur PSIM, il se peut que les résultats ne concordent plus avec les autres simulateurs</t>
   </si>
   <si>
-    <t>Tester le simulateur sur le plus différentes versions de PSIM</t>
-  </si>
-  <si>
     <t>Responsable du risque</t>
   </si>
   <si>
@@ -138,6 +129,15 @@
   </si>
   <si>
     <t>Le simulateur ne s'amorçe plus correctement, les affichages ne sont plus fonctionnels, les données ne concordent plus</t>
+  </si>
+  <si>
+    <t>Faire des tests à partir de différentes plateformes et à partir de différents systèmes d'exploitation de manière à s'assurer l'homogénéité dans le fonctionnement de Matlab</t>
+  </si>
+  <si>
+    <t>Tester le simulateur sur le plus de versions différentes de PSIM</t>
+  </si>
+  <si>
+    <t>S'assurer de bien maintenir les révisions à jour, travaille collaboratif mis fréquemment à jour et dont les changements sont réversibles au moyen d'une synchronisation sur un serveur web protégé (GitHub)</t>
   </si>
 </sst>
 </file>
@@ -237,12 +237,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -268,10 +272,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="7">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -571,10 +583,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -608,7 +620,7 @@
         <v>11</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="66" customHeight="1" thickTop="1">
@@ -674,7 +686,7 @@
         <v>0.2</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>22</v>
+        <v>33</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>14</v>
@@ -682,22 +694,22 @@
     </row>
     <row r="5" spans="1:7" ht="154">
       <c r="A5" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B5" s="1">
         <v>4</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>24</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>25</v>
       </c>
       <c r="E5" s="3">
         <v>0.15</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="G5" s="1" t="s">
         <v>14</v>
@@ -705,22 +717,22 @@
     </row>
     <row r="6" spans="1:7" ht="98">
       <c r="A6" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B6" s="1">
         <v>3</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E6" s="3">
         <v>0.1</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="G6" s="1" t="s">
         <v>4</v>
@@ -736,16 +748,36 @@
       <c r="C7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>33</v>
+      <c r="D7" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="E7" s="3">
         <v>0.2</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="G7" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="D11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="D12" s="9">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="D13" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="D14" t="s">
         <v>3</v>
       </c>
     </row>

</xml_diff>